<commit_message>
I got my EDA done. I need to add a row sum column
</commit_message>
<xml_diff>
--- a/CH-088 Subtotal Calculation.xlsx
+++ b/CH-088 Subtotal Calculation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFF042E4-635F-4C18-8C40-22C25A315E86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C5AA857-60C1-4FAE-9D32-26BBDFE1F803}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="17">
   <si>
     <t>Question</t>
   </si>
@@ -2157,8 +2157,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{426F43EE-6285-45A2-8AEA-346E58770E6B}">
   <dimension ref="A1:P47"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="O37" sqref="O37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2835,6 +2835,25 @@
       <c r="E26" t="str">
         <v>Region 2</v>
       </c>
+      <c r="F26" t="s">
+        <v>15</v>
+      </c>
+      <c r="H26" t="b" cm="1">
+        <f t="array" ref="H26:L47">B26:F47=I2:M23</f>
+        <v>1</v>
+      </c>
+      <c r="I26" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J26" t="b">
+        <v>1</v>
+      </c>
+      <c r="K26" t="b">
+        <v>1</v>
+      </c>
+      <c r="L26" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="str">
@@ -2849,6 +2868,25 @@
       <c r="E27">
         <v>50</v>
       </c>
+      <c r="F27">
+        <f>SUM(D27:E27)</f>
+        <v>100</v>
+      </c>
+      <c r="H27" t="b">
+        <v>1</v>
+      </c>
+      <c r="I27" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J27" t="b">
+        <v>1</v>
+      </c>
+      <c r="K27" t="b">
+        <v>1</v>
+      </c>
+      <c r="L27" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B28" s="4" t="str">
@@ -2863,6 +2901,25 @@
       <c r="E28">
         <v>13</v>
       </c>
+      <c r="F28">
+        <f t="shared" ref="F28:F47" si="0">SUM(D28:E28)</f>
+        <v>27</v>
+      </c>
+      <c r="H28" t="b">
+        <v>1</v>
+      </c>
+      <c r="I28" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J28" t="b">
+        <v>1</v>
+      </c>
+      <c r="K28" t="b">
+        <v>1</v>
+      </c>
+      <c r="L28" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="str">
@@ -2877,6 +2934,25 @@
       <c r="E29">
         <v>38</v>
       </c>
+      <c r="F29">
+        <f t="shared" si="0"/>
+        <v>74</v>
+      </c>
+      <c r="H29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I29" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J29" t="b">
+        <v>1</v>
+      </c>
+      <c r="K29" t="b">
+        <v>1</v>
+      </c>
+      <c r="L29" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B30" s="4" t="str">
@@ -2891,6 +2967,25 @@
       <c r="E30">
         <v>36</v>
       </c>
+      <c r="F30">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+      <c r="H30" t="b">
+        <v>1</v>
+      </c>
+      <c r="I30" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J30" t="b">
+        <v>1</v>
+      </c>
+      <c r="K30" t="b">
+        <v>1</v>
+      </c>
+      <c r="L30" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B31" s="4" t="str">
@@ -2905,6 +3000,25 @@
       <c r="E31">
         <v>137</v>
       </c>
+      <c r="F31">
+        <f t="shared" si="0"/>
+        <v>260</v>
+      </c>
+      <c r="H31" t="b">
+        <v>0</v>
+      </c>
+      <c r="I31" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J31" t="b">
+        <v>1</v>
+      </c>
+      <c r="K31" t="b">
+        <v>1</v>
+      </c>
+      <c r="L31" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B32" s="4" t="str">
@@ -2919,8 +3033,27 @@
       <c r="E32">
         <v>26</v>
       </c>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F32">
+        <f t="shared" si="0"/>
+        <v>71</v>
+      </c>
+      <c r="H32" t="b">
+        <v>1</v>
+      </c>
+      <c r="I32" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J32" t="b">
+        <v>1</v>
+      </c>
+      <c r="K32" t="b">
+        <v>1</v>
+      </c>
+      <c r="L32" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B33" s="4" t="str">
         <v>B</v>
       </c>
@@ -2933,8 +3066,27 @@
       <c r="E33">
         <v>12</v>
       </c>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F33">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="H33" t="b">
+        <v>1</v>
+      </c>
+      <c r="I33" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J33" t="b">
+        <v>1</v>
+      </c>
+      <c r="K33" t="b">
+        <v>1</v>
+      </c>
+      <c r="L33" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B34" s="4" t="str">
         <v>B</v>
       </c>
@@ -2947,8 +3099,27 @@
       <c r="E34">
         <v>48</v>
       </c>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F34">
+        <f t="shared" si="0"/>
+        <v>97</v>
+      </c>
+      <c r="H34" t="b">
+        <v>1</v>
+      </c>
+      <c r="I34" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J34" t="b">
+        <v>1</v>
+      </c>
+      <c r="K34" t="b">
+        <v>1</v>
+      </c>
+      <c r="L34" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B35" s="4" t="str">
         <v>B</v>
       </c>
@@ -2961,8 +3132,27 @@
       <c r="E35">
         <v>39</v>
       </c>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F35">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="H35" t="b">
+        <v>1</v>
+      </c>
+      <c r="I35" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J35" t="b">
+        <v>1</v>
+      </c>
+      <c r="K35" t="b">
+        <v>1</v>
+      </c>
+      <c r="L35" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B36" s="4" t="str">
         <v>B</v>
       </c>
@@ -2975,8 +3165,27 @@
       <c r="E36">
         <v>125</v>
       </c>
-    </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F36">
+        <f t="shared" si="0"/>
+        <v>291</v>
+      </c>
+      <c r="H36" t="b">
+        <v>0</v>
+      </c>
+      <c r="I36" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J36" t="b">
+        <v>1</v>
+      </c>
+      <c r="K36" t="b">
+        <v>1</v>
+      </c>
+      <c r="L36" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B37" s="4" t="str">
         <v>C</v>
       </c>
@@ -2989,8 +3198,27 @@
       <c r="E37">
         <v>25</v>
       </c>
-    </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F37">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+      <c r="H37" t="b">
+        <v>1</v>
+      </c>
+      <c r="I37" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J37" t="b">
+        <v>1</v>
+      </c>
+      <c r="K37" t="b">
+        <v>1</v>
+      </c>
+      <c r="L37" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B38" s="4" t="str">
         <v>C</v>
       </c>
@@ -3003,8 +3231,27 @@
       <c r="E38">
         <v>49</v>
       </c>
-    </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F38">
+        <f t="shared" si="0"/>
+        <v>71</v>
+      </c>
+      <c r="H38" t="b">
+        <v>1</v>
+      </c>
+      <c r="I38" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J38" t="b">
+        <v>1</v>
+      </c>
+      <c r="K38" t="b">
+        <v>1</v>
+      </c>
+      <c r="L38" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B39" s="4" t="str">
         <v>C</v>
       </c>
@@ -3017,8 +3264,27 @@
       <c r="E39">
         <v>39</v>
       </c>
-    </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F39">
+        <f t="shared" si="0"/>
+        <v>74</v>
+      </c>
+      <c r="H39" t="b">
+        <v>1</v>
+      </c>
+      <c r="I39" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J39" t="b">
+        <v>1</v>
+      </c>
+      <c r="K39" t="b">
+        <v>1</v>
+      </c>
+      <c r="L39" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B40" s="4" t="str">
         <v>C</v>
       </c>
@@ -3031,8 +3297,27 @@
       <c r="E40">
         <v>27</v>
       </c>
-    </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F40">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="H40" t="b">
+        <v>1</v>
+      </c>
+      <c r="I40" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J40" t="b">
+        <v>1</v>
+      </c>
+      <c r="K40" t="b">
+        <v>1</v>
+      </c>
+      <c r="L40" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B41" s="4" t="str">
         <v>C</v>
       </c>
@@ -3045,8 +3330,27 @@
       <c r="E41">
         <v>140</v>
       </c>
-    </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F41">
+        <f t="shared" si="0"/>
+        <v>248</v>
+      </c>
+      <c r="H41" t="b">
+        <v>0</v>
+      </c>
+      <c r="I41" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J41" t="b">
+        <v>1</v>
+      </c>
+      <c r="K41" t="b">
+        <v>1</v>
+      </c>
+      <c r="L41" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B42" s="4" t="str">
         <v>D</v>
       </c>
@@ -3059,8 +3363,27 @@
       <c r="E42">
         <v>27</v>
       </c>
-    </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F42">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+      <c r="H42" t="b">
+        <v>1</v>
+      </c>
+      <c r="I42" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J42" t="b">
+        <v>1</v>
+      </c>
+      <c r="K42" t="b">
+        <v>1</v>
+      </c>
+      <c r="L42" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B43" s="4" t="str">
         <v>D</v>
       </c>
@@ -3073,8 +3396,27 @@
       <c r="E43">
         <v>29</v>
       </c>
-    </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F43">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="H43" t="b">
+        <v>1</v>
+      </c>
+      <c r="I43" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J43" t="b">
+        <v>1</v>
+      </c>
+      <c r="K43" t="b">
+        <v>1</v>
+      </c>
+      <c r="L43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B44" s="4" t="str">
         <v>D</v>
       </c>
@@ -3087,8 +3429,27 @@
       <c r="E44">
         <v>48</v>
       </c>
-    </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F44">
+        <f t="shared" si="0"/>
+        <v>95</v>
+      </c>
+      <c r="H44" t="b">
+        <v>1</v>
+      </c>
+      <c r="I44" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J44" t="b">
+        <v>1</v>
+      </c>
+      <c r="K44" t="b">
+        <v>1</v>
+      </c>
+      <c r="L44" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B45" s="4" t="str">
         <v>D</v>
       </c>
@@ -3101,8 +3462,27 @@
       <c r="E45">
         <v>18</v>
       </c>
-    </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F45">
+        <f t="shared" si="0"/>
+        <v>61</v>
+      </c>
+      <c r="H45" t="b">
+        <v>1</v>
+      </c>
+      <c r="I45" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J45" t="b">
+        <v>1</v>
+      </c>
+      <c r="K45" t="b">
+        <v>1</v>
+      </c>
+      <c r="L45" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B46" s="4" t="str">
         <v>D</v>
       </c>
@@ -3115,8 +3495,27 @@
       <c r="E46">
         <v>122</v>
       </c>
-    </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F46">
+        <f t="shared" si="0"/>
+        <v>254</v>
+      </c>
+      <c r="H46" t="b">
+        <v>0</v>
+      </c>
+      <c r="I46" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J46" t="b">
+        <v>1</v>
+      </c>
+      <c r="K46" t="b">
+        <v>1</v>
+      </c>
+      <c r="L46" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B47" s="4" t="str">
         <v>Grand Total</v>
       </c>
@@ -3128,6 +3527,25 @@
       </c>
       <c r="E47">
         <v>524</v>
+      </c>
+      <c r="F47">
+        <f t="shared" si="0"/>
+        <v>1053</v>
+      </c>
+      <c r="H47" t="b">
+        <v>1</v>
+      </c>
+      <c r="I47" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J47" t="b">
+        <v>1</v>
+      </c>
+      <c r="K47" t="b">
+        <v>1</v>
+      </c>
+      <c r="L47" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -3145,7 +3563,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D167758-7207-4E19-A73D-25779201F538}">
   <dimension ref="A1:P47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="O35" sqref="O35"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
I think I got the single function done
</commit_message>
<xml_diff>
--- a/CH-088 Subtotal Calculation.xlsx
+++ b/CH-088 Subtotal Calculation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C5AA857-60C1-4FAE-9D32-26BBDFE1F803}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25CEFE7C-119E-42E2-BFC5-323C3A7C4733}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
@@ -18,13 +18,16 @@
     <sheet name="Alt1" sheetId="3" r:id="rId3"/>
     <sheet name="Alt2" sheetId="5" r:id="rId4"/>
     <sheet name="Alt3" sheetId="6" r:id="rId5"/>
+    <sheet name="MySingle" sheetId="8" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Alt1'!$B$2:$D$18</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Alt2'!$B$2:$D$18</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Alt3'!$B$2:$D$18</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">EDA!$B$2:$D$18</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">MySingle!$B$2:$D$18</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Original!$B$2:$D$18</definedName>
+    <definedName name="HD_Date">_xlfn.LET(_xlpm.dt, TODAY(),      _xlpm.y,  YEAR(_xlpm.dt),      _xlpm.m,  MONTH(_xlpm.dt),      _xlpm.d,  DAY(_xlpm.dt),      TEXT(DATE(_xlpm.y,_xlpm.m,_xlpm.d),"dd-mmm-yyyy")     )</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -69,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="17">
   <si>
     <t>Question</t>
   </si>
@@ -129,7 +132,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dddd"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -157,8 +160,23 @@
       <family val="1"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -180,6 +198,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59996337778862885"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -426,8 +456,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -536,8 +568,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Intro_Hd" xfId="2" xr:uid="{0A05A210-99C9-4D51-A85E-0B691D4ED418}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{841CC4EA-2015-4673-83FB-1CCCC1BAF325}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1197,6 +1231,135 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>79375</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>342899</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>155575</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle: Rounded Corners 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1CC332E1-46A3-418C-B5E2-25E9827E1309}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3220720" y="361315"/>
+          <a:ext cx="1747519" cy="2354580"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-AU" sz="1600" b="1">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Challenge 88: Subtotal Calculation!</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:br>
+            <a:rPr lang="en-AU" sz="1400" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-AU" sz="1400" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>In the question table, sales info provided.</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-AU" sz="1400" b="1" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t> Add subtotals and grand total into the data like result table.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-AU" sz="1400" b="1">
+            <a:solidFill>
+              <a:srgbClr val="FFC000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Wisp">
   <a:themeElements>
@@ -2157,8 +2320,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{426F43EE-6285-45A2-8AEA-346E58770E6B}">
   <dimension ref="A1:P47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="O37" sqref="O37"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -3563,7 +3726,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D167758-7207-4E19-A73D-25779201F538}">
   <dimension ref="A1:P47"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="O35" sqref="O35"/>
     </sheetView>
   </sheetViews>
@@ -6028,7 +6191,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAD3BB6C-6144-4934-80B9-B52AD5F2A56D}">
   <dimension ref="A1:P44"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
+    <sheetView topLeftCell="A21" workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
@@ -7062,4 +7225,1391 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C029030E-923F-406D-879A-791D65B60C5C}">
+  <dimension ref="A1:P47"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26:F47"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.09765625" customWidth="1"/>
+    <col min="2" max="4" width="9.5" style="4" customWidth="1"/>
+    <col min="5" max="5" width="9.5" customWidth="1"/>
+    <col min="6" max="6" width="12.19921875" customWidth="1"/>
+    <col min="7" max="7" width="7.3984375" customWidth="1"/>
+    <col min="8" max="8" width="5.09765625" customWidth="1"/>
+    <col min="9" max="9" width="11.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.3984375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" s="8" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="36"/>
+      <c r="I1" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="17"/>
+    </row>
+    <row r="2" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="I2" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" s="22" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="13">
+        <v>1</v>
+      </c>
+      <c r="D3" s="13">
+        <v>50</v>
+      </c>
+      <c r="E3" s="13">
+        <v>50</v>
+      </c>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="I3" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="24">
+        <v>1</v>
+      </c>
+      <c r="K3" s="24">
+        <v>50</v>
+      </c>
+      <c r="L3" s="24">
+        <v>50</v>
+      </c>
+      <c r="M3" s="33">
+        <v>100</v>
+      </c>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="9"/>
+    </row>
+    <row r="4" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="13">
+        <v>2</v>
+      </c>
+      <c r="D4" s="13">
+        <v>14</v>
+      </c>
+      <c r="E4" s="13">
+        <v>13</v>
+      </c>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="I4" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="J4" s="24">
+        <v>2</v>
+      </c>
+      <c r="K4" s="24">
+        <v>14</v>
+      </c>
+      <c r="L4" s="24">
+        <v>13</v>
+      </c>
+      <c r="M4" s="33">
+        <v>27</v>
+      </c>
+      <c r="N4" s="11"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="9"/>
+    </row>
+    <row r="5" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="13">
+        <v>3</v>
+      </c>
+      <c r="D5" s="13">
+        <v>36</v>
+      </c>
+      <c r="E5" s="13">
+        <v>38</v>
+      </c>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="I5" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="J5" s="24">
+        <v>3</v>
+      </c>
+      <c r="K5" s="24">
+        <v>36</v>
+      </c>
+      <c r="L5" s="24">
+        <v>38</v>
+      </c>
+      <c r="M5" s="33">
+        <v>74</v>
+      </c>
+      <c r="N5" s="11"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="9"/>
+    </row>
+    <row r="6" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="13">
+        <v>4</v>
+      </c>
+      <c r="D6" s="13">
+        <v>23</v>
+      </c>
+      <c r="E6" s="13">
+        <v>36</v>
+      </c>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="I6" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="J6" s="24">
+        <v>4</v>
+      </c>
+      <c r="K6" s="24">
+        <v>23</v>
+      </c>
+      <c r="L6" s="24">
+        <v>36</v>
+      </c>
+      <c r="M6" s="33">
+        <v>59</v>
+      </c>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="9"/>
+    </row>
+    <row r="7" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="13">
+        <v>1</v>
+      </c>
+      <c r="D7" s="13">
+        <v>45</v>
+      </c>
+      <c r="E7" s="13">
+        <v>26</v>
+      </c>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="I7" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="J7" s="26"/>
+      <c r="K7" s="27">
+        <v>123</v>
+      </c>
+      <c r="L7" s="27">
+        <v>137</v>
+      </c>
+      <c r="M7" s="28">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="13">
+        <v>2</v>
+      </c>
+      <c r="D8" s="13">
+        <v>31</v>
+      </c>
+      <c r="E8" s="13">
+        <v>12</v>
+      </c>
+      <c r="F8"/>
+      <c r="G8"/>
+      <c r="H8"/>
+      <c r="I8" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="J8" s="24">
+        <v>1</v>
+      </c>
+      <c r="K8" s="24">
+        <v>45</v>
+      </c>
+      <c r="L8" s="24">
+        <v>26</v>
+      </c>
+      <c r="M8" s="33">
+        <v>71</v>
+      </c>
+      <c r="N8"/>
+      <c r="O8"/>
+      <c r="P8"/>
+    </row>
+    <row r="9" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="13">
+        <v>3</v>
+      </c>
+      <c r="D9" s="13">
+        <v>49</v>
+      </c>
+      <c r="E9" s="13">
+        <v>48</v>
+      </c>
+      <c r="F9"/>
+      <c r="G9"/>
+      <c r="H9"/>
+      <c r="I9" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="J9" s="24">
+        <v>2</v>
+      </c>
+      <c r="K9" s="24">
+        <v>31</v>
+      </c>
+      <c r="L9" s="24">
+        <v>12</v>
+      </c>
+      <c r="M9" s="33">
+        <v>43</v>
+      </c>
+      <c r="N9"/>
+      <c r="O9"/>
+      <c r="P9"/>
+    </row>
+    <row r="10" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="13">
+        <v>4</v>
+      </c>
+      <c r="D10" s="13">
+        <v>41</v>
+      </c>
+      <c r="E10" s="13">
+        <v>39</v>
+      </c>
+      <c r="F10"/>
+      <c r="G10"/>
+      <c r="H10"/>
+      <c r="I10" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="J10" s="24">
+        <v>3</v>
+      </c>
+      <c r="K10" s="24">
+        <v>49</v>
+      </c>
+      <c r="L10" s="24">
+        <v>48</v>
+      </c>
+      <c r="M10" s="33">
+        <v>97</v>
+      </c>
+      <c r="N10"/>
+      <c r="O10"/>
+      <c r="P10"/>
+    </row>
+    <row r="11" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="13">
+        <v>1</v>
+      </c>
+      <c r="D11" s="13">
+        <v>26</v>
+      </c>
+      <c r="E11" s="13">
+        <v>25</v>
+      </c>
+      <c r="F11"/>
+      <c r="G11"/>
+      <c r="H11"/>
+      <c r="I11" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="J11" s="24">
+        <v>4</v>
+      </c>
+      <c r="K11" s="24">
+        <v>41</v>
+      </c>
+      <c r="L11" s="24">
+        <v>39</v>
+      </c>
+      <c r="M11" s="33">
+        <v>80</v>
+      </c>
+      <c r="N11"/>
+      <c r="O11"/>
+      <c r="P11"/>
+    </row>
+    <row r="12" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="13">
+        <v>2</v>
+      </c>
+      <c r="D12" s="13">
+        <v>22</v>
+      </c>
+      <c r="E12" s="13">
+        <v>49</v>
+      </c>
+      <c r="F12"/>
+      <c r="G12"/>
+      <c r="H12"/>
+      <c r="I12" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="J12" s="26"/>
+      <c r="K12" s="27">
+        <v>166</v>
+      </c>
+      <c r="L12" s="27">
+        <v>125</v>
+      </c>
+      <c r="M12" s="28">
+        <v>291</v>
+      </c>
+      <c r="N12"/>
+      <c r="O12"/>
+      <c r="P12"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B13" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="13">
+        <v>3</v>
+      </c>
+      <c r="D13" s="13">
+        <v>35</v>
+      </c>
+      <c r="E13" s="13">
+        <v>39</v>
+      </c>
+      <c r="I13" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="J13" s="24">
+        <v>1</v>
+      </c>
+      <c r="K13" s="24">
+        <v>26</v>
+      </c>
+      <c r="L13" s="24">
+        <v>25</v>
+      </c>
+      <c r="M13" s="33">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B14" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="13">
+        <v>4</v>
+      </c>
+      <c r="D14" s="13">
+        <v>25</v>
+      </c>
+      <c r="E14" s="13">
+        <v>27</v>
+      </c>
+      <c r="I14" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="J14" s="24">
+        <v>2</v>
+      </c>
+      <c r="K14" s="24">
+        <v>22</v>
+      </c>
+      <c r="L14" s="24">
+        <v>49</v>
+      </c>
+      <c r="M14" s="33">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="13">
+        <v>1</v>
+      </c>
+      <c r="D15" s="13">
+        <v>26</v>
+      </c>
+      <c r="E15" s="13">
+        <v>27</v>
+      </c>
+      <c r="I15" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="J15" s="24">
+        <v>3</v>
+      </c>
+      <c r="K15" s="24">
+        <v>35</v>
+      </c>
+      <c r="L15" s="24">
+        <v>39</v>
+      </c>
+      <c r="M15" s="33">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="13">
+        <v>2</v>
+      </c>
+      <c r="D16" s="13">
+        <v>16</v>
+      </c>
+      <c r="E16" s="13">
+        <v>29</v>
+      </c>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="I16" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="J16" s="24">
+        <v>4</v>
+      </c>
+      <c r="K16" s="24">
+        <v>25</v>
+      </c>
+      <c r="L16" s="24">
+        <v>27</v>
+      </c>
+      <c r="M16" s="33">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="13">
+        <v>3</v>
+      </c>
+      <c r="D17" s="13">
+        <v>47</v>
+      </c>
+      <c r="E17" s="13">
+        <v>48</v>
+      </c>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="I17" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="J17" s="26"/>
+      <c r="K17" s="27">
+        <v>108</v>
+      </c>
+      <c r="L17" s="27">
+        <v>140</v>
+      </c>
+      <c r="M17" s="28">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="14">
+        <v>4</v>
+      </c>
+      <c r="D18" s="14">
+        <v>43</v>
+      </c>
+      <c r="E18" s="14">
+        <v>18</v>
+      </c>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="I18" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="J18" s="24">
+        <v>1</v>
+      </c>
+      <c r="K18" s="24">
+        <v>26</v>
+      </c>
+      <c r="L18" s="24">
+        <v>27</v>
+      </c>
+      <c r="M18" s="33">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I19" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="J19" s="24">
+        <v>2</v>
+      </c>
+      <c r="K19" s="24">
+        <v>16</v>
+      </c>
+      <c r="L19" s="24">
+        <v>29</v>
+      </c>
+      <c r="M19" s="33">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I20" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="J20" s="24">
+        <v>3</v>
+      </c>
+      <c r="K20" s="24">
+        <v>47</v>
+      </c>
+      <c r="L20" s="24">
+        <v>48</v>
+      </c>
+      <c r="M20" s="33">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I21" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="J21" s="24">
+        <v>4</v>
+      </c>
+      <c r="K21" s="24">
+        <v>43</v>
+      </c>
+      <c r="L21" s="24">
+        <v>18</v>
+      </c>
+      <c r="M21" s="33">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I22" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="J22" s="29"/>
+      <c r="K22" s="27">
+        <v>132</v>
+      </c>
+      <c r="L22" s="27">
+        <v>122</v>
+      </c>
+      <c r="M22" s="28">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I23" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="J23" s="30"/>
+      <c r="K23" s="31">
+        <v>529</v>
+      </c>
+      <c r="L23" s="31">
+        <v>524</v>
+      </c>
+      <c r="M23" s="32">
+        <v>1053</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B26" s="20" t="str" cm="1">
+        <f t="array" ref="B26:F47">_xlfn.LET(
+_xlpm.x, _xlfn.GROUPBY(B2:C18, D2:E18, _xleta.SUM, 3, 2),
+_xlpm.y, _xlfn.LET(_xlpm.z,_xlfn.BYROW(_xlpm.x,_xlfn.LAMBDA(_xlpm.r,SUM(INDEX(_xlpm.r,,{3,4})))),IF(_xlpm.z=0,"Total Regions",_xlpm.z)),_xlfn.HSTACK(_xlpm.x,_xlpm.y))</f>
+        <v>Product</v>
+      </c>
+      <c r="C26" s="21" t="str">
+        <v>Season</v>
+      </c>
+      <c r="D26" s="21" t="str">
+        <v>Region 1</v>
+      </c>
+      <c r="E26" s="21" t="str">
+        <v>Region 2</v>
+      </c>
+      <c r="F26" s="22" t="str">
+        <v>Total Regions</v>
+      </c>
+      <c r="H26" t="b" cm="1">
+        <f t="array" ref="H26:L47">B26:F47=I2:M23</f>
+        <v>1</v>
+      </c>
+      <c r="I26" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J26" t="b">
+        <v>1</v>
+      </c>
+      <c r="K26" t="b">
+        <v>1</v>
+      </c>
+      <c r="L26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B27" s="23" t="str">
+        <v>A</v>
+      </c>
+      <c r="C27" s="24">
+        <v>1</v>
+      </c>
+      <c r="D27" s="24">
+        <v>50</v>
+      </c>
+      <c r="E27" s="24">
+        <v>50</v>
+      </c>
+      <c r="F27" s="33">
+        <v>100</v>
+      </c>
+      <c r="H27" t="b">
+        <v>1</v>
+      </c>
+      <c r="I27" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J27" t="b">
+        <v>1</v>
+      </c>
+      <c r="K27" t="b">
+        <v>1</v>
+      </c>
+      <c r="L27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B28" s="23" t="str">
+        <v>A</v>
+      </c>
+      <c r="C28" s="24">
+        <v>2</v>
+      </c>
+      <c r="D28" s="24">
+        <v>14</v>
+      </c>
+      <c r="E28" s="24">
+        <v>13</v>
+      </c>
+      <c r="F28" s="33">
+        <v>27</v>
+      </c>
+      <c r="H28" t="b">
+        <v>1</v>
+      </c>
+      <c r="I28" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J28" t="b">
+        <v>1</v>
+      </c>
+      <c r="K28" t="b">
+        <v>1</v>
+      </c>
+      <c r="L28" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B29" s="23" t="str">
+        <v>A</v>
+      </c>
+      <c r="C29" s="24">
+        <v>3</v>
+      </c>
+      <c r="D29" s="24">
+        <v>36</v>
+      </c>
+      <c r="E29" s="24">
+        <v>38</v>
+      </c>
+      <c r="F29" s="33">
+        <v>74</v>
+      </c>
+      <c r="H29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I29" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J29" t="b">
+        <v>1</v>
+      </c>
+      <c r="K29" t="b">
+        <v>1</v>
+      </c>
+      <c r="L29" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B30" s="23" t="str">
+        <v>A</v>
+      </c>
+      <c r="C30" s="24">
+        <v>4</v>
+      </c>
+      <c r="D30" s="24">
+        <v>23</v>
+      </c>
+      <c r="E30" s="24">
+        <v>36</v>
+      </c>
+      <c r="F30" s="33">
+        <v>59</v>
+      </c>
+      <c r="H30" t="b">
+        <v>1</v>
+      </c>
+      <c r="I30" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J30" t="b">
+        <v>1</v>
+      </c>
+      <c r="K30" t="b">
+        <v>1</v>
+      </c>
+      <c r="L30" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B31" s="25" t="str">
+        <v>A</v>
+      </c>
+      <c r="C31" s="26" t="str">
+        <v/>
+      </c>
+      <c r="D31" s="27">
+        <v>123</v>
+      </c>
+      <c r="E31" s="27">
+        <v>137</v>
+      </c>
+      <c r="F31" s="28">
+        <v>260</v>
+      </c>
+      <c r="H31" t="b">
+        <v>0</v>
+      </c>
+      <c r="I31" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J31" t="b">
+        <v>1</v>
+      </c>
+      <c r="K31" t="b">
+        <v>1</v>
+      </c>
+      <c r="L31" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B32" s="23" t="str">
+        <v>B</v>
+      </c>
+      <c r="C32" s="24">
+        <v>1</v>
+      </c>
+      <c r="D32" s="24">
+        <v>45</v>
+      </c>
+      <c r="E32" s="24">
+        <v>26</v>
+      </c>
+      <c r="F32" s="33">
+        <v>71</v>
+      </c>
+      <c r="H32" t="b">
+        <v>1</v>
+      </c>
+      <c r="I32" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J32" t="b">
+        <v>1</v>
+      </c>
+      <c r="K32" t="b">
+        <v>1</v>
+      </c>
+      <c r="L32" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B33" s="23" t="str">
+        <v>B</v>
+      </c>
+      <c r="C33" s="24">
+        <v>2</v>
+      </c>
+      <c r="D33" s="24">
+        <v>31</v>
+      </c>
+      <c r="E33" s="24">
+        <v>12</v>
+      </c>
+      <c r="F33" s="33">
+        <v>43</v>
+      </c>
+      <c r="H33" t="b">
+        <v>1</v>
+      </c>
+      <c r="I33" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J33" t="b">
+        <v>1</v>
+      </c>
+      <c r="K33" t="b">
+        <v>1</v>
+      </c>
+      <c r="L33" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B34" s="23" t="str">
+        <v>B</v>
+      </c>
+      <c r="C34" s="24">
+        <v>3</v>
+      </c>
+      <c r="D34" s="24">
+        <v>49</v>
+      </c>
+      <c r="E34" s="24">
+        <v>48</v>
+      </c>
+      <c r="F34" s="33">
+        <v>97</v>
+      </c>
+      <c r="H34" t="b">
+        <v>1</v>
+      </c>
+      <c r="I34" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J34" t="b">
+        <v>1</v>
+      </c>
+      <c r="K34" t="b">
+        <v>1</v>
+      </c>
+      <c r="L34" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B35" s="23" t="str">
+        <v>B</v>
+      </c>
+      <c r="C35" s="24">
+        <v>4</v>
+      </c>
+      <c r="D35" s="24">
+        <v>41</v>
+      </c>
+      <c r="E35" s="24">
+        <v>39</v>
+      </c>
+      <c r="F35" s="33">
+        <v>80</v>
+      </c>
+      <c r="H35" t="b">
+        <v>1</v>
+      </c>
+      <c r="I35" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J35" t="b">
+        <v>1</v>
+      </c>
+      <c r="K35" t="b">
+        <v>1</v>
+      </c>
+      <c r="L35" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B36" s="25" t="str">
+        <v>B</v>
+      </c>
+      <c r="C36" s="26" t="str">
+        <v/>
+      </c>
+      <c r="D36" s="27">
+        <v>166</v>
+      </c>
+      <c r="E36" s="27">
+        <v>125</v>
+      </c>
+      <c r="F36" s="28">
+        <v>291</v>
+      </c>
+      <c r="H36" t="b">
+        <v>0</v>
+      </c>
+      <c r="I36" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J36" t="b">
+        <v>1</v>
+      </c>
+      <c r="K36" t="b">
+        <v>1</v>
+      </c>
+      <c r="L36" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B37" s="23" t="str">
+        <v>C</v>
+      </c>
+      <c r="C37" s="24">
+        <v>1</v>
+      </c>
+      <c r="D37" s="24">
+        <v>26</v>
+      </c>
+      <c r="E37" s="24">
+        <v>25</v>
+      </c>
+      <c r="F37" s="33">
+        <v>51</v>
+      </c>
+      <c r="H37" t="b">
+        <v>1</v>
+      </c>
+      <c r="I37" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J37" t="b">
+        <v>1</v>
+      </c>
+      <c r="K37" t="b">
+        <v>1</v>
+      </c>
+      <c r="L37" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B38" s="23" t="str">
+        <v>C</v>
+      </c>
+      <c r="C38" s="24">
+        <v>2</v>
+      </c>
+      <c r="D38" s="24">
+        <v>22</v>
+      </c>
+      <c r="E38" s="24">
+        <v>49</v>
+      </c>
+      <c r="F38" s="33">
+        <v>71</v>
+      </c>
+      <c r="H38" t="b">
+        <v>1</v>
+      </c>
+      <c r="I38" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J38" t="b">
+        <v>1</v>
+      </c>
+      <c r="K38" t="b">
+        <v>1</v>
+      </c>
+      <c r="L38" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B39" s="23" t="str">
+        <v>C</v>
+      </c>
+      <c r="C39" s="24">
+        <v>3</v>
+      </c>
+      <c r="D39" s="24">
+        <v>35</v>
+      </c>
+      <c r="E39" s="24">
+        <v>39</v>
+      </c>
+      <c r="F39" s="33">
+        <v>74</v>
+      </c>
+      <c r="H39" t="b">
+        <v>1</v>
+      </c>
+      <c r="I39" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J39" t="b">
+        <v>1</v>
+      </c>
+      <c r="K39" t="b">
+        <v>1</v>
+      </c>
+      <c r="L39" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B40" s="23" t="str">
+        <v>C</v>
+      </c>
+      <c r="C40" s="24">
+        <v>4</v>
+      </c>
+      <c r="D40" s="24">
+        <v>25</v>
+      </c>
+      <c r="E40" s="24">
+        <v>27</v>
+      </c>
+      <c r="F40" s="33">
+        <v>52</v>
+      </c>
+      <c r="H40" t="b">
+        <v>1</v>
+      </c>
+      <c r="I40" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J40" t="b">
+        <v>1</v>
+      </c>
+      <c r="K40" t="b">
+        <v>1</v>
+      </c>
+      <c r="L40" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B41" s="25" t="str">
+        <v>C</v>
+      </c>
+      <c r="C41" s="26" t="str">
+        <v/>
+      </c>
+      <c r="D41" s="27">
+        <v>108</v>
+      </c>
+      <c r="E41" s="27">
+        <v>140</v>
+      </c>
+      <c r="F41" s="28">
+        <v>248</v>
+      </c>
+      <c r="H41" t="b">
+        <v>0</v>
+      </c>
+      <c r="I41" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J41" t="b">
+        <v>1</v>
+      </c>
+      <c r="K41" t="b">
+        <v>1</v>
+      </c>
+      <c r="L41" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B42" s="23" t="str">
+        <v>D</v>
+      </c>
+      <c r="C42" s="24">
+        <v>1</v>
+      </c>
+      <c r="D42" s="24">
+        <v>26</v>
+      </c>
+      <c r="E42" s="24">
+        <v>27</v>
+      </c>
+      <c r="F42" s="33">
+        <v>53</v>
+      </c>
+      <c r="H42" t="b">
+        <v>1</v>
+      </c>
+      <c r="I42" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J42" t="b">
+        <v>1</v>
+      </c>
+      <c r="K42" t="b">
+        <v>1</v>
+      </c>
+      <c r="L42" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B43" s="23" t="str">
+        <v>D</v>
+      </c>
+      <c r="C43" s="24">
+        <v>2</v>
+      </c>
+      <c r="D43" s="24">
+        <v>16</v>
+      </c>
+      <c r="E43" s="24">
+        <v>29</v>
+      </c>
+      <c r="F43" s="33">
+        <v>45</v>
+      </c>
+      <c r="H43" t="b">
+        <v>1</v>
+      </c>
+      <c r="I43" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J43" t="b">
+        <v>1</v>
+      </c>
+      <c r="K43" t="b">
+        <v>1</v>
+      </c>
+      <c r="L43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B44" s="23" t="str">
+        <v>D</v>
+      </c>
+      <c r="C44" s="24">
+        <v>3</v>
+      </c>
+      <c r="D44" s="24">
+        <v>47</v>
+      </c>
+      <c r="E44" s="24">
+        <v>48</v>
+      </c>
+      <c r="F44" s="33">
+        <v>95</v>
+      </c>
+      <c r="H44" t="b">
+        <v>1</v>
+      </c>
+      <c r="I44" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J44" t="b">
+        <v>1</v>
+      </c>
+      <c r="K44" t="b">
+        <v>1</v>
+      </c>
+      <c r="L44" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B45" s="23" t="str">
+        <v>D</v>
+      </c>
+      <c r="C45" s="24">
+        <v>4</v>
+      </c>
+      <c r="D45" s="24">
+        <v>43</v>
+      </c>
+      <c r="E45" s="24">
+        <v>18</v>
+      </c>
+      <c r="F45" s="33">
+        <v>61</v>
+      </c>
+      <c r="H45" t="b">
+        <v>1</v>
+      </c>
+      <c r="I45" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J45" t="b">
+        <v>1</v>
+      </c>
+      <c r="K45" t="b">
+        <v>1</v>
+      </c>
+      <c r="L45" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B46" s="18" t="str">
+        <v>D</v>
+      </c>
+      <c r="C46" s="29" t="str">
+        <v/>
+      </c>
+      <c r="D46" s="27">
+        <v>132</v>
+      </c>
+      <c r="E46" s="27">
+        <v>122</v>
+      </c>
+      <c r="F46" s="28">
+        <v>254</v>
+      </c>
+      <c r="H46" t="b">
+        <v>0</v>
+      </c>
+      <c r="I46" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J46" t="b">
+        <v>1</v>
+      </c>
+      <c r="K46" t="b">
+        <v>1</v>
+      </c>
+      <c r="L46" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B47" s="19" t="str">
+        <v>Grand Total</v>
+      </c>
+      <c r="C47" s="30" t="str">
+        <v/>
+      </c>
+      <c r="D47" s="31">
+        <v>529</v>
+      </c>
+      <c r="E47" s="31">
+        <v>524</v>
+      </c>
+      <c r="F47" s="32">
+        <v>1053</v>
+      </c>
+      <c r="H47" t="b">
+        <v>1</v>
+      </c>
+      <c r="I47" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J47" t="b">
+        <v>1</v>
+      </c>
+      <c r="K47" t="b">
+        <v>1</v>
+      </c>
+      <c r="L47" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="I1:L1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
I am trying to figure out why the other solutions are so complex
</commit_message>
<xml_diff>
--- a/CH-088 Subtotal Calculation.xlsx
+++ b/CH-088 Subtotal Calculation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25CEFE7C-119E-42E2-BFC5-323C3A7C4733}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FF6A880-002C-4ABC-8DD5-4E2EB10F1D35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="19">
   <si>
     <t>Question</t>
   </si>
@@ -123,6 +123,12 @@
   </si>
   <si>
     <t>https://www.linkedin.com/feed/update/urn:li:activity:7222344872421122048/</t>
+  </si>
+  <si>
+    <t>I do not understand why other folks have more complex solutions.</t>
+  </si>
+  <si>
+    <t>Clearly, I am missing something.</t>
   </si>
 </sst>
 </file>
@@ -176,7 +182,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -198,12 +204,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -459,9 +459,9 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -566,6 +566,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -7229,10 +7232,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C029030E-923F-406D-879A-791D65B60C5C}">
-  <dimension ref="A1:P47"/>
+  <dimension ref="A1:P51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26:F47"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="J52" sqref="J52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -8603,6 +8606,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B50" s="39" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B51" s="39" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:E1"/>

</xml_diff>

<commit_message>
Got the single function figured out. I also understand why all the solutions are complex
</commit_message>
<xml_diff>
--- a/CH-088 Subtotal Calculation.xlsx
+++ b/CH-088 Subtotal Calculation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FF6A880-002C-4ABC-8DD5-4E2EB10F1D35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75BC3C52-A01A-4B26-B593-97BBD5E572C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="18">
   <si>
     <t>Question</t>
   </si>
@@ -125,10 +125,7 @@
     <t>https://www.linkedin.com/feed/update/urn:li:activity:7222344872421122048/</t>
   </si>
   <si>
-    <t>I do not understand why other folks have more complex solutions.</t>
-  </si>
-  <si>
-    <t>Clearly, I am missing something.</t>
+    <t xml:space="preserve">Okay, I am getting there. The issue is now in the first column. </t>
   </si>
 </sst>
 </file>
@@ -461,7 +458,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -569,6 +566,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -7232,10 +7241,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C029030E-923F-406D-879A-791D65B60C5C}">
-  <dimension ref="A1:P51"/>
+  <dimension ref="A1:P53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="J52" sqref="J52"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -7245,7 +7254,7 @@
     <col min="5" max="5" width="9.5" customWidth="1"/>
     <col min="6" max="6" width="12.19921875" customWidth="1"/>
     <col min="7" max="7" width="7.3984375" customWidth="1"/>
-    <col min="8" max="8" width="5.09765625" customWidth="1"/>
+    <col min="8" max="8" width="6.5" customWidth="1"/>
     <col min="9" max="9" width="11.5" style="6" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14.3984375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
@@ -7902,7 +7911,12 @@
       <c r="B26" s="20" t="str" cm="1">
         <f t="array" ref="B26:F47">_xlfn.LET(
 _xlpm.x, _xlfn.GROUPBY(B2:C18, D2:E18, _xleta.SUM, 3, 2),
-_xlpm.y, _xlfn.LET(_xlpm.z,_xlfn.BYROW(_xlpm.x,_xlfn.LAMBDA(_xlpm.r,SUM(INDEX(_xlpm.r,,{3,4})))),IF(_xlpm.z=0,"Total Regions",_xlpm.z)),_xlfn.HSTACK(_xlpm.x,_xlpm.y))</f>
+_xlpm.y, _xlfn.LET(_xlpm.z,_xlfn.BYROW(_xlpm.x,_xlfn.LAMBDA(_xlpm.r,SUM(INDEX(_xlpm.r,,{3,4})))),IF(_xlpm.z=0,"Total Regions",_xlpm.z)),
+_xlpm.z, _xlfn.HSTACK(_xlpm.x,_xlpm.y),
+_xlpm.zz, _xlfn.CHOOSECOLS(_xlpm.z,1,2),
+_xlpm.zzz,_xlfn.BYROW(_xlpm.zz,
+          _xlfn.LAMBDA(_xlpm.r,IF(AND(LEN(INDEX(_xlpm.r,,2))=0,
+                       NOT(ISNUMBER(FIND("Grand",INDEX(_xlpm.r,,1))))),"Total "&amp;INDEX(_xlpm.r,,1),INDEX(_xlpm.r,,1)))),_xlfn.HSTACK(_xlpm.zzz,_xlfn.DROP(_xlpm.z,,1)))</f>
         <v>Product</v>
       </c>
       <c r="C26" s="21" t="str">
@@ -7935,7 +7949,7 @@
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B27" s="23" t="str">
+      <c r="B27" s="40" t="str">
         <v>A</v>
       </c>
       <c r="C27" s="24">
@@ -7967,7 +7981,7 @@
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B28" s="23" t="str">
+      <c r="B28" s="40" t="str">
         <v>A</v>
       </c>
       <c r="C28" s="24">
@@ -7999,7 +8013,7 @@
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B29" s="23" t="str">
+      <c r="B29" s="40" t="str">
         <v>A</v>
       </c>
       <c r="C29" s="24">
@@ -8031,7 +8045,7 @@
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B30" s="23" t="str">
+      <c r="B30" s="40" t="str">
         <v>A</v>
       </c>
       <c r="C30" s="24">
@@ -8063,8 +8077,8 @@
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B31" s="25" t="str">
-        <v>A</v>
+      <c r="B31" s="41" t="str">
+        <v>Total A</v>
       </c>
       <c r="C31" s="26" t="str">
         <v/>
@@ -8079,23 +8093,27 @@
         <v>260</v>
       </c>
       <c r="H31" t="b">
+        <v>1</v>
+      </c>
+      <c r="I31" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J31" t="b">
+        <v>1</v>
+      </c>
+      <c r="K31" t="b">
+        <v>1</v>
+      </c>
+      <c r="L31" t="b">
+        <v>1</v>
+      </c>
+      <c r="M31">
+        <f>LEN(C31)</f>
         <v>0</v>
       </c>
-      <c r="I31" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="J31" t="b">
-        <v>1</v>
-      </c>
-      <c r="K31" t="b">
-        <v>1</v>
-      </c>
-      <c r="L31" t="b">
-        <v>1</v>
-      </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B32" s="23" t="str">
+      <c r="B32" s="40" t="str">
         <v>B</v>
       </c>
       <c r="C32" s="24">
@@ -8127,7 +8145,7 @@
       </c>
     </row>
     <row r="33" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B33" s="23" t="str">
+      <c r="B33" s="40" t="str">
         <v>B</v>
       </c>
       <c r="C33" s="24">
@@ -8159,7 +8177,7 @@
       </c>
     </row>
     <row r="34" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B34" s="23" t="str">
+      <c r="B34" s="40" t="str">
         <v>B</v>
       </c>
       <c r="C34" s="24">
@@ -8191,7 +8209,7 @@
       </c>
     </row>
     <row r="35" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B35" s="23" t="str">
+      <c r="B35" s="40" t="str">
         <v>B</v>
       </c>
       <c r="C35" s="24">
@@ -8223,8 +8241,8 @@
       </c>
     </row>
     <row r="36" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B36" s="25" t="str">
-        <v>B</v>
+      <c r="B36" s="41" t="str">
+        <v>Total B</v>
       </c>
       <c r="C36" s="26" t="str">
         <v/>
@@ -8239,7 +8257,7 @@
         <v>291</v>
       </c>
       <c r="H36" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I36" s="6" t="b">
         <v>1</v>
@@ -8255,7 +8273,7 @@
       </c>
     </row>
     <row r="37" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B37" s="23" t="str">
+      <c r="B37" s="40" t="str">
         <v>C</v>
       </c>
       <c r="C37" s="24">
@@ -8287,7 +8305,7 @@
       </c>
     </row>
     <row r="38" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B38" s="23" t="str">
+      <c r="B38" s="40" t="str">
         <v>C</v>
       </c>
       <c r="C38" s="24">
@@ -8319,7 +8337,7 @@
       </c>
     </row>
     <row r="39" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B39" s="23" t="str">
+      <c r="B39" s="40" t="str">
         <v>C</v>
       </c>
       <c r="C39" s="24">
@@ -8351,7 +8369,7 @@
       </c>
     </row>
     <row r="40" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B40" s="23" t="str">
+      <c r="B40" s="40" t="str">
         <v>C</v>
       </c>
       <c r="C40" s="24">
@@ -8383,8 +8401,8 @@
       </c>
     </row>
     <row r="41" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B41" s="25" t="str">
-        <v>C</v>
+      <c r="B41" s="41" t="str">
+        <v>Total C</v>
       </c>
       <c r="C41" s="26" t="str">
         <v/>
@@ -8399,7 +8417,7 @@
         <v>248</v>
       </c>
       <c r="H41" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I41" s="6" t="b">
         <v>1</v>
@@ -8415,7 +8433,7 @@
       </c>
     </row>
     <row r="42" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B42" s="23" t="str">
+      <c r="B42" s="40" t="str">
         <v>D</v>
       </c>
       <c r="C42" s="24">
@@ -8447,7 +8465,7 @@
       </c>
     </row>
     <row r="43" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B43" s="23" t="str">
+      <c r="B43" s="40" t="str">
         <v>D</v>
       </c>
       <c r="C43" s="24">
@@ -8479,7 +8497,7 @@
       </c>
     </row>
     <row r="44" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B44" s="23" t="str">
+      <c r="B44" s="40" t="str">
         <v>D</v>
       </c>
       <c r="C44" s="24">
@@ -8511,7 +8529,7 @@
       </c>
     </row>
     <row r="45" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B45" s="23" t="str">
+      <c r="B45" s="40" t="str">
         <v>D</v>
       </c>
       <c r="C45" s="24">
@@ -8543,8 +8561,8 @@
       </c>
     </row>
     <row r="46" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B46" s="18" t="str">
-        <v>D</v>
+      <c r="B46" s="42" t="str">
+        <v>Total D</v>
       </c>
       <c r="C46" s="29" t="str">
         <v/>
@@ -8559,7 +8577,7 @@
         <v>254</v>
       </c>
       <c r="H46" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I46" s="6" t="b">
         <v>1</v>
@@ -8575,7 +8593,7 @@
       </c>
     </row>
     <row r="47" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B47" s="19" t="str">
+      <c r="B47" s="43" t="str">
         <v>Grand Total</v>
       </c>
       <c r="C47" s="30" t="str">
@@ -8607,13 +8625,14 @@
       </c>
     </row>
     <row r="50" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B50" s="39" t="s">
+      <c r="B50" s="39"/>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B51" s="39"/>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B53" s="4" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B51" s="39" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>